<commit_message>
Correction des fautes d'horographe
</commit_message>
<xml_diff>
--- a/Doccument_théorique/Scénarios.xlsx
+++ b/Doccument_théorique/Scénarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\BatailleNavale\Doccument_théorique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83c501277422d836/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3CE818-3A5C-4FA9-AD76-4AA3F3FBA276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75BA5AFB-3E82-4536-B8D7-5CB36FC9A7F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8880" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>Cas:</t>
   </si>
@@ -48,148 +48,139 @@
     <t>Réaction</t>
   </si>
   <si>
-    <t>Lance le jeu</t>
-  </si>
-  <si>
-    <t>Lance une partie</t>
-  </si>
-  <si>
-    <t>Insère des coordonée</t>
-  </si>
-  <si>
-    <t>Les coordonée sont elles valide ?</t>
-  </si>
-  <si>
-    <t>oui</t>
-  </si>
-  <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>Repose la question</t>
-  </si>
-  <si>
-    <t>Il y a encore des bateau ?</t>
-  </si>
-  <si>
-    <t>Retourn a "insère des coordonée</t>
-  </si>
-  <si>
-    <t>Affiche l'écran de fin</t>
-  </si>
-  <si>
-    <t>Montre le tableau des scores</t>
-  </si>
-  <si>
-    <t>"système pause"</t>
-  </si>
-  <si>
     <t>Cas :</t>
   </si>
   <si>
-    <t>Affiche les règle</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
-    <t>Va dans règle</t>
-  </si>
-  <si>
-    <t>Affiche le menu des règle</t>
-  </si>
-  <si>
     <t>"Système pause"</t>
   </si>
   <si>
     <t>S'authentifier</t>
   </si>
   <si>
-    <t>Rentre ton pseudo</t>
-  </si>
-  <si>
-    <t>si il est trop grand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repose la question </t>
-  </si>
-  <si>
-    <t>si ok</t>
-  </si>
-  <si>
-    <t>Enregistre le nom</t>
-  </si>
-  <si>
-    <t>Affiche un message de confirmation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Si presse n </t>
   </si>
   <si>
-    <t>si presse o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repose la question </t>
-  </si>
-  <si>
-    <t>Affiche le menu des scores</t>
-  </si>
-  <si>
-    <t>Demande le menu des scores</t>
-  </si>
-  <si>
-    <t>Affiche le menu des score</t>
-  </si>
-  <si>
     <t>Retour au menu</t>
   </si>
   <si>
-    <t>Choisis de s'identifier</t>
-  </si>
-  <si>
-    <t>Regarde la case</t>
-  </si>
-  <si>
-    <t>il y a un bateau ?</t>
-  </si>
-  <si>
     <t>Oui</t>
   </si>
   <si>
-    <t>Marque la case en rouge</t>
-  </si>
-  <si>
-    <t>Demare le programme</t>
-  </si>
-  <si>
-    <t>Demande de s'dentifier</t>
-  </si>
-  <si>
-    <t>il presse non</t>
-  </si>
-  <si>
-    <t>il presse oui</t>
-  </si>
-  <si>
-    <t>scénario S'authentifier</t>
-  </si>
-  <si>
-    <t>Scénario Jouer</t>
-  </si>
-  <si>
-    <t>Appuie sur enter</t>
-  </si>
-  <si>
-    <t>Ecrit 1 et appuie sur enter</t>
-  </si>
-  <si>
-    <t>Ecrit 2 et appuie sur enter</t>
-  </si>
-  <si>
-    <t>Affiche la grille</t>
-  </si>
-  <si>
-    <t>Marque la case en bleu</t>
+    <t>Lancer le jeu</t>
+  </si>
+  <si>
+    <t>Scénario -&gt; s'authentifier</t>
+  </si>
+  <si>
+    <t>Aller dans règle</t>
+  </si>
+  <si>
+    <t>Scénario -&gt; jouer</t>
+  </si>
+  <si>
+    <t>Rentrer son pseudo</t>
+  </si>
+  <si>
+    <t>Demander le menu des scores</t>
+  </si>
+  <si>
+    <t>Démarrer le programme</t>
+  </si>
+  <si>
+    <t>Ecrire 1 et appuyer sur enter</t>
+  </si>
+  <si>
+    <t>Insérer des coordonées</t>
+  </si>
+  <si>
+    <t>Appyier sur enter</t>
+  </si>
+  <si>
+    <t>Ecrire 2 et appuyer sur enter</t>
+  </si>
+  <si>
+    <t>Appuyer sur enter</t>
+  </si>
+  <si>
+    <t>Choisir de s'identifier</t>
+  </si>
+  <si>
+    <t>Les coordonées sont-elles valides ?</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Y a-t-il un bateau ?</t>
+  </si>
+  <si>
+    <t>Y a-t-il encore des bateaux ?</t>
+  </si>
+  <si>
+    <t>Afficher les règles</t>
+  </si>
+  <si>
+    <t>Presser non</t>
+  </si>
+  <si>
+    <t>Presser oui</t>
+  </si>
+  <si>
+    <t>S'il est trop grand</t>
+  </si>
+  <si>
+    <t>Si ok</t>
+  </si>
+  <si>
+    <t>Si presse o</t>
+  </si>
+  <si>
+    <t>Afficher le menu des scores</t>
+  </si>
+  <si>
+    <t>Lancer une partie</t>
+  </si>
+  <si>
+    <t>Afficher la grille</t>
+  </si>
+  <si>
+    <t>Reposer la question</t>
+  </si>
+  <si>
+    <t>Regarder la case</t>
+  </si>
+  <si>
+    <t>Marquer la case en bleu</t>
+  </si>
+  <si>
+    <t>Marquer la case en rouge</t>
+  </si>
+  <si>
+    <t>Retourner à "insérer des coordonées"</t>
+  </si>
+  <si>
+    <t>Afficher l'écran de fin</t>
+  </si>
+  <si>
+    <t>Montrer le tableau des scores</t>
+  </si>
+  <si>
+    <t>Afficher le menu des règles</t>
+  </si>
+  <si>
+    <t>Demander de s'identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reposer la question </t>
+  </si>
+  <si>
+    <t>Afficher un message de confirmation</t>
+  </si>
+  <si>
+    <t>Enregistrer le nom</t>
   </si>
 </sst>
 </file>
@@ -570,18 +561,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -590,331 +581,331 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
         <v>46</v>
       </c>
-      <c r="D34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>